<commit_message>
changed data to mlm in route in app.py
</commit_message>
<xml_diff>
--- a/support_docs/Neural_Net_Performance.xlsx
+++ b/support_docs/Neural_Net_Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Brown\Desktop\Team5_FinalProject\support_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F800811-9BBB-489E-8D5B-1C1BFEBD9004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC7E0C2-7449-4EF5-85B0-50F8F45DC1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{069F6B91-0C53-4E7B-AEF6-9988D4EE306E}"/>
+    <workbookView xWindow="3810" yWindow="1930" windowWidth="9600" windowHeight="4910" firstSheet="2" activeTab="6" xr2:uid="{069F6B91-0C53-4E7B-AEF6-9988D4EE306E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Optimization" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="73">
   <si>
     <t>Layer 1</t>
   </si>
@@ -257,6 +257,9 @@
   <si>
     <t>Adadelta</t>
   </si>
+  <si>
+    <t>running analysis test on smote data of 57048 data points</t>
+  </si>
 </sst>
 </file>
 
@@ -427,13 +430,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8753,15 +8756,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>545647</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>67808</xdr:rowOff>
+      <xdr:colOff>528865</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>10204</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>240847</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>90033</xdr:rowOff>
+      <xdr:colOff>224065</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>32429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8789,15 +8792,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>567644</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>10657</xdr:rowOff>
+      <xdr:colOff>550862</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>143553</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>262844</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>51253</xdr:rowOff>
+      <xdr:colOff>246062</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>7256</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9257,7 +9260,7 @@
   <dimension ref="A3:AD210"/>
   <sheetViews>
     <sheetView topLeftCell="P7" workbookViewId="0">
-      <pane ySplit="1440" topLeftCell="A40" activePane="bottomLeft"/>
+      <pane ySplit="1450" topLeftCell="A40" activePane="bottomLeft"/>
       <selection activeCell="U3" sqref="U3:AD3"/>
       <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
@@ -9279,10 +9282,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="R3" s="35" t="s">
+      <c r="R3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="35"/>
+      <c r="S3" s="36"/>
       <c r="U3" s="2" t="s">
         <v>25</v>
       </c>
@@ -26427,22 +26430,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="36"/>
+      <c r="I3" s="37"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
@@ -42266,28 +42269,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="35"/>
+      <c r="S3" s="36"/>
       <c r="T3" s="13"/>
       <c r="U3" s="9" t="s">
         <v>25</v>
@@ -45558,10 +45561,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC0A1CD-5C2D-4A58-A5B1-71EA28D777A4}">
-  <dimension ref="A4:X34"/>
+  <dimension ref="A4:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45573,6 +45576,9 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" t="s">
         <v>51</v>
       </c>
@@ -46403,6 +46409,38 @@
       <c r="H18">
         <v>0.23</v>
       </c>
+      <c r="P18">
+        <f>SUM(Q18:T18)</f>
+        <v>57048</v>
+      </c>
+      <c r="Q18">
+        <v>28203</v>
+      </c>
+      <c r="R18">
+        <v>27683</v>
+      </c>
+      <c r="S18">
+        <v>841</v>
+      </c>
+      <c r="T18">
+        <v>321</v>
+      </c>
+      <c r="U18" s="21">
+        <f t="shared" ref="U18" si="25">(Q18+R18)/P18</f>
+        <v>0.979631187771701</v>
+      </c>
+      <c r="V18" s="21">
+        <f t="shared" ref="V18" si="26">IF(AND(Q18=0, S18=0),0,(Q18/(Q18+S18)))</f>
+        <v>0.97104393334251482</v>
+      </c>
+      <c r="W18" s="21">
+        <f t="shared" ref="W18" si="27">(Q18/(Q18+T18))</f>
+        <v>0.98874631888935638</v>
+      </c>
+      <c r="X18" s="21">
+        <f t="shared" ref="X18" si="28">IF(AND(V18=0,W18=0),0,2*(V18*W18)/(V18+W18))</f>
+        <v>0.97981517509727623</v>
+      </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -46429,6 +46467,38 @@
       <c r="H19">
         <v>0.14000000000000001</v>
       </c>
+      <c r="P19">
+        <f>SUM(Q19:T19)</f>
+        <v>57048</v>
+      </c>
+      <c r="Q19">
+        <v>27925</v>
+      </c>
+      <c r="R19">
+        <v>26920</v>
+      </c>
+      <c r="S19">
+        <v>1604</v>
+      </c>
+      <c r="T19">
+        <v>599</v>
+      </c>
+      <c r="U19" s="21">
+        <f t="shared" ref="U19" si="29">(Q19+R19)/P19</f>
+        <v>0.96138339643808723</v>
+      </c>
+      <c r="V19" s="21">
+        <f t="shared" ref="V19" si="30">IF(AND(Q19=0, S19=0),0,(Q19/(Q19+S19)))</f>
+        <v>0.94568051745741477</v>
+      </c>
+      <c r="W19" s="21">
+        <f t="shared" ref="W19" si="31">(Q19/(Q19+T19))</f>
+        <v>0.97900014023278648</v>
+      </c>
+      <c r="X19" s="21">
+        <f t="shared" ref="X19" si="32">IF(AND(V19=0,W19=0),0,2*(V19*W19)/(V19+W19))</f>
+        <v>0.96205191807486257</v>
+      </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -46649,7 +46719,7 @@
       <c r="D27" s="27">
         <v>100</v>
       </c>
-      <c r="E27" s="37">
+      <c r="E27" s="35">
         <v>1000</v>
       </c>
       <c r="F27" s="27" t="s">
@@ -46855,7 +46925,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>28524</v>
       </c>
@@ -46890,7 +46960,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>28524</v>
       </c>
@@ -46923,6 +46993,93 @@
       </c>
       <c r="L34">
         <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>28524</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>100</v>
+      </c>
+      <c r="E35" s="32">
+        <v>1000</v>
+      </c>
+      <c r="F35" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35">
+        <v>0.98</v>
+      </c>
+      <c r="I35">
+        <v>28203</v>
+      </c>
+      <c r="J35">
+        <v>27683</v>
+      </c>
+      <c r="K35">
+        <v>841</v>
+      </c>
+      <c r="L35">
+        <v>321</v>
+      </c>
+      <c r="M35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>28524</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36" s="32">
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H36">
+        <v>0.96</v>
+      </c>
+      <c r="I36">
+        <v>27925</v>
+      </c>
+      <c r="J36">
+        <v>26920</v>
+      </c>
+      <c r="K36">
+        <v>1604</v>
+      </c>
+      <c r="L36">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>28524</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>55</v>
+      </c>
+      <c r="E37" s="32">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
machine learn page updated and model switched to random forest
</commit_message>
<xml_diff>
--- a/support_docs/Neural_Net_Performance.xlsx
+++ b/support_docs/Neural_Net_Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Brown\Desktop\Team5_FinalProject\support_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545A5F1A-564B-411E-B867-DAE06FC108AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E46CB8-43AF-456B-A845-8B80D1A8D598}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{069F6B91-0C53-4E7B-AEF6-9988D4EE306E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{069F6B91-0C53-4E7B-AEF6-9988D4EE306E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Optimization" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Plots" sheetId="3" r:id="rId5"/>
     <sheet name="SMOTE Comparison" sheetId="6" r:id="rId6"/>
     <sheet name="Optimizer" sheetId="7" r:id="rId7"/>
+    <sheet name="Results" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3102" uniqueCount="80">
   <si>
     <t>Layer 1</t>
   </si>
@@ -260,6 +261,27 @@
   <si>
     <t>running analysis test on smote data of 57048 data points</t>
   </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Total samples: 57048</t>
+  </si>
+  <si>
+    <t>True Positive: 27429</t>
+  </si>
+  <si>
+    <t>True Negative: 26457</t>
+  </si>
+  <si>
+    <t>False Positive: 2067</t>
+  </si>
+  <si>
+    <t>False Negative: 1095</t>
+  </si>
 </sst>
 </file>
 
@@ -268,7 +290,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +312,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -346,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,8 +462,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8755,16 +8789,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>528865</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>10204</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>171905</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>143100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>224065</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>32429</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>506640</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>165325</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8791,16 +8825,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>550862</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>143553</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>142648</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>126772</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>246062</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>7256</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>477383</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>173717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9260,7 +9294,7 @@
   <dimension ref="A3:AD210"/>
   <sheetViews>
     <sheetView topLeftCell="P7" workbookViewId="0">
-      <pane ySplit="1440" topLeftCell="A40" activePane="bottomLeft"/>
+      <pane ySplit="2030" topLeftCell="A40" activePane="bottomLeft"/>
       <selection activeCell="U3" sqref="U3:AD3"/>
       <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
@@ -9282,10 +9316,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="R3" s="36" t="s">
+      <c r="R3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="36"/>
+      <c r="S3" s="37"/>
       <c r="U3" s="2" t="s">
         <v>25</v>
       </c>
@@ -26430,22 +26464,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="37"/>
+      <c r="I3" s="38"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
@@ -42269,28 +42303,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="36"/>
+      <c r="S3" s="37"/>
       <c r="T3" s="13"/>
       <c r="U3" s="9" t="s">
         <v>25</v>
@@ -45561,10 +45595,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC0A1CD-5C2D-4A58-A5B1-71EA28D777A4}">
-  <dimension ref="A4:X37"/>
+  <dimension ref="A4:X45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -46484,19 +46518,19 @@
         <v>599</v>
       </c>
       <c r="U19" s="21">
-        <f t="shared" ref="U19" si="29">(Q19+R19)/P19</f>
+        <f t="shared" ref="U19:U21" si="29">(Q19+R19)/P19</f>
         <v>0.96138339643808723</v>
       </c>
       <c r="V19" s="21">
-        <f t="shared" ref="V19" si="30">IF(AND(Q19=0, S19=0),0,(Q19/(Q19+S19)))</f>
+        <f t="shared" ref="V19:V21" si="30">IF(AND(Q19=0, S19=0),0,(Q19/(Q19+S19)))</f>
         <v>0.94568051745741477</v>
       </c>
       <c r="W19" s="21">
-        <f t="shared" ref="W19" si="31">(Q19/(Q19+T19))</f>
+        <f t="shared" ref="W19:W21" si="31">(Q19/(Q19+T19))</f>
         <v>0.97900014023278648</v>
       </c>
       <c r="X19" s="21">
-        <f t="shared" ref="X19" si="32">IF(AND(V19=0,W19=0),0,2*(V19*W19)/(V19+W19))</f>
+        <f t="shared" ref="X19:X21" si="32">IF(AND(V19=0,W19=0),0,2*(V19*W19)/(V19+W19))</f>
         <v>0.96205191807486257</v>
       </c>
     </row>
@@ -46525,6 +46559,38 @@
       <c r="H20">
         <v>0.27</v>
       </c>
+      <c r="P20">
+        <f>SUM(Q20:T20)</f>
+        <v>57048</v>
+      </c>
+      <c r="Q20">
+        <v>27429</v>
+      </c>
+      <c r="R20">
+        <v>26457</v>
+      </c>
+      <c r="S20">
+        <v>2067</v>
+      </c>
+      <c r="T20">
+        <v>1095</v>
+      </c>
+      <c r="U20" s="21">
+        <f t="shared" si="29"/>
+        <v>0.94457299116533444</v>
+      </c>
+      <c r="V20" s="21">
+        <f t="shared" si="30"/>
+        <v>0.9299227013832384</v>
+      </c>
+      <c r="W20" s="21">
+        <f t="shared" si="31"/>
+        <v>0.96161127471602859</v>
+      </c>
+      <c r="X20" s="21">
+        <f t="shared" si="32"/>
+        <v>0.94550155118924495</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -46551,6 +46617,38 @@
       <c r="H21">
         <v>0.37</v>
       </c>
+      <c r="P21">
+        <f>SUM(Q21:T21)</f>
+        <v>29072</v>
+      </c>
+      <c r="Q21">
+        <v>64</v>
+      </c>
+      <c r="R21">
+        <v>28501</v>
+      </c>
+      <c r="S21">
+        <v>23</v>
+      </c>
+      <c r="T21">
+        <v>484</v>
+      </c>
+      <c r="U21" s="21">
+        <f t="shared" si="29"/>
+        <v>0.98256053935057786</v>
+      </c>
+      <c r="V21" s="21">
+        <f t="shared" si="30"/>
+        <v>0.73563218390804597</v>
+      </c>
+      <c r="W21" s="21">
+        <f t="shared" si="31"/>
+        <v>0.11678832116788321</v>
+      </c>
+      <c r="X21" s="21">
+        <f t="shared" si="32"/>
+        <v>0.2015748031496063</v>
+      </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -46925,7 +47023,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>28524</v>
       </c>
@@ -46960,7 +47058,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>28524</v>
       </c>
@@ -46995,7 +47093,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>28524</v>
       </c>
@@ -47033,7 +47131,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>28524</v>
       </c>
@@ -47068,7 +47166,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>28524</v>
       </c>
@@ -47080,10 +47178,87 @@
       </c>
       <c r="E37" s="32">
         <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q41" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q42" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q43" s="39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q44" s="39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="Q45" s="39" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491CD696-5280-42D9-9EDC-A149406060E4}">
+  <dimension ref="D4:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="E4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D5" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D6" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D10" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>